<commit_message>
ajuste para validacion de cargue de productos por medio de archivo excel, se valida existencia de nombres, sku, codigo barras y tipo de dato numericos
</commit_message>
<xml_diff>
--- a/archivos/Cargue masivo/Productos con exitencias/ProductoStock.xlsx
+++ b/archivos/Cargue masivo/Productos con exitencias/ProductoStock.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Sku</t>
   </si>
@@ -45,21 +45,6 @@
   </si>
   <si>
     <t>Stock *</t>
-  </si>
-  <si>
-    <t>teclado</t>
-  </si>
-  <si>
-    <t>mause</t>
-  </si>
-  <si>
-    <t>puerta</t>
-  </si>
-  <si>
-    <t>hp</t>
-  </si>
-  <si>
-    <t>logict</t>
   </si>
 </sst>
 </file>
@@ -462,7 +447,7 @@
   <dimension ref="A1:G2875"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -498,52 +483,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="14">
-        <v>0</v>
-      </c>
-      <c r="F2" s="14">
-        <v>42500</v>
-      </c>
-      <c r="G2" s="14">
-        <v>5</v>
-      </c>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="14">
-        <v>10000</v>
-      </c>
-      <c r="F3" s="14">
-        <v>20000</v>
-      </c>
-      <c r="G3" s="14">
-        <v>10</v>
-      </c>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="14">
-        <v>0</v>
-      </c>
-      <c r="F4" s="14">
-        <v>150000</v>
-      </c>
-      <c r="G4" s="14">
-        <v>4</v>
-      </c>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>

</xml_diff>

<commit_message>
Se agregan ajustes necesario para generacion de factura electronica y avances en generacion de nota credito electronica
</commit_message>
<xml_diff>
--- a/archivos/Cargue masivo/Productos con exitencias/ProductoStock.xlsx
+++ b/archivos/Cargue masivo/Productos con exitencias/ProductoStock.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Sku</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Stock *</t>
+  </si>
+  <si>
+    <t>Impuesto % *</t>
   </si>
 </sst>
 </file>
@@ -444,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2875"/>
+  <dimension ref="A1:H2875"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -457,9 +460,10 @@
     <col min="4" max="4" width="18.140625" style="1" customWidth="1"/>
     <col min="5" max="6" width="25.28515625" style="14" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" style="14"/>
+    <col min="8" max="8" width="14.28515625" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -481,50 +485,53 @@
       <c r="G1" s="13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Avance inclusion de tributos iva, inc, inc bolsa
</commit_message>
<xml_diff>
--- a/archivos/Cargue masivo/Productos con exitencias/ProductoStock.xlsx
+++ b/archivos/Cargue masivo/Productos con exitencias/ProductoStock.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Sku</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Impuesto % *</t>
+  </si>
+  <si>
+    <t>Tributo (IVA, INC)</t>
   </si>
 </sst>
 </file>
@@ -132,7 +135,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -166,6 +169,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -447,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2875"/>
+  <dimension ref="A1:I2875"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -461,9 +465,10 @@
     <col min="5" max="6" width="25.28515625" style="14" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" style="14"/>
     <col min="8" max="8" width="14.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -488,50 +493,53 @@
       <c r="H1" s="13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Se agrega tributos iva, inc y inc bolsa en facturas y notas credito local
</commit_message>
<xml_diff>
--- a/archivos/Cargue masivo/Productos con exitencias/ProductoStock.xlsx
+++ b/archivos/Cargue masivo/Productos con exitencias/ProductoStock.xlsx
@@ -60,7 +60,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +91,14 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -135,7 +143,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -170,6 +178,7 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -454,7 +463,7 @@
   <dimension ref="A1:I2875"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -499,6 +508,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2" s="1"/>
+      <c r="I2" s="16"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="2"/>

</xml_diff>